<commit_message>
Complete Light and Camera Mount
</commit_message>
<xml_diff>
--- a/doc/BOM.xlsx
+++ b/doc/BOM.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -468,260 +468,514 @@
         <v/>
       </c>
     </row>
-    <row r="4">
-      <c r="D4" t="str">
+    <row r="5">
+      <c r="D5" t="str">
         <v>Raspberry Pi 4B 4GB</v>
       </c>
-      <c r="E4" t="str">
+      <c r="E5" t="str">
         <v>Raspberry Pi to handle the system, possess USB ports, GPIO, CSI Camera. May need a seperate GPU for inferencing</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F5" t="str">
         <v>45</v>
       </c>
-      <c r="G4" t="str">
+      <c r="G5" t="str">
         <v>https://onecall.farnell.com/raspberry-pi/rpi4-modbp-4gb/raspberry-pi-4-model-b-4gb/dp/3051887</v>
       </c>
-      <c r="H4" t="str">
+      <c r="H5" t="str">
         <v>RPI</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="str">
+      <c r="I5" t="str">
+        <v>45.46</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="D6" t="str">
+        <v>Okdo ROCK 4 Model C+</v>
+      </c>
+      <c r="E6" t="str">
+        <v>RPi alternative with all the same inputs and outputs</v>
+      </c>
+      <c r="F6" t="str">
+        <v>45</v>
+      </c>
+      <c r="G6" t="str">
+        <v>https://uk.rs-online.com/web/p/rock-sbc-boards/2493158?intcmp=UK-WEB-_-CP-FP1-_-Dec-22-_-okdo-rock-single-4cplus</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="str">
         <v>GPU Processor</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C7" t="str">
         <v>Seperate modules that provide AI inferencing capabilities</v>
       </c>
     </row>
-    <row r="6">
-      <c r="D6" t="str">
+    <row r="8">
+      <c r="D8" t="str">
         <v>Intel Neural Compute Stick</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E8" t="str">
         <v>Provides real time inferencing capabilties to the raspberry pi</v>
       </c>
-      <c r="F6" t="str">
+      <c r="F8" t="str">
         <v>59</v>
       </c>
-      <c r="G6" t="str">
+      <c r="G8" t="str">
         <v>https://uk.rs-online.com/web/p/processor-development-tools/1393655?gb=s</v>
       </c>
-      <c r="H6" t="str">
+      <c r="H8" t="str">
         <v>RPI</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
+    <row r="9">
+      <c r="A9" t="str">
         <v>Vision</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B9" t="str">
         <v>CSI Camera</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C9" t="str">
         <v>Camera used for the visionn system</v>
       </c>
     </row>
-    <row r="8">
-      <c r="C8" t="str">
+    <row r="10">
+      <c r="C10" t="str">
         <v/>
       </c>
-      <c r="D8" t="str">
+      <c r="D10" t="str">
         <v>OV5647 Camera Adjustable Focus</v>
       </c>
-      <c r="E8" t="str">
+      <c r="E10" t="str">
         <v>Adjustable focus camera, allows for macro shots</v>
       </c>
-      <c r="F8" t="str">
+      <c r="F10" t="str">
         <v>6</v>
       </c>
-      <c r="G8" t="str">
+      <c r="G10" t="str">
         <v>https://www.aliexpress.com/item/1005003386791483.html?spm=a2g0o.productlist.main.1.189a245aZHaLsB&amp;algo_pvid=260a6382-35b3-4d7e-86af-53e171ab5e10&amp;algo_exp_id=260a6382-35b3-4d7e-86af-53e171ab5e10-0&amp;pdp_npi=4%40dis%21GBP%215.45%215.45%21%21%216.50%21%21%40211b443e16995361090023304ee15b%2112000027225320432%21sea%21UK%211802951889%21&amp;curPageLogUid=gnYNy1UG26o0</v>
       </c>
-      <c r="J8" t="str">
+      <c r="H10" t="str">
+        <v>CAM</v>
+      </c>
+      <c r="J10" t="str">
         <v>Used here: https://www.instructables.com/RPi-MacroScope/</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="C9" t="str">
-        <v/>
-      </c>
-      <c r="D9" t="str">
-        <v>Ribbon Extension Cable</v>
-      </c>
-      <c r="E9" t="str">
-        <v>300mm cable</v>
-      </c>
-      <c r="F9" t="str">
-        <v>1.20</v>
-      </c>
-      <c r="G9" t="str">
-        <v>https://onecall.farnell.com/pro-signal/ctlcamcableassy-300mm/cable-for-pi-camera-300mm-formed/dp/SC13282?st=camera%20ribbon</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="D10" t="str">
-        <v>SD Card</v>
-      </c>
-      <c r="E10" t="str">
-        <v>32GB UHS-I U1 V10</v>
-      </c>
-      <c r="F10" t="str">
-        <v>8.30</v>
-      </c>
-      <c r="G10" t="str">
-        <v>https://onecall.farnell.com/integral/inmsdh32g10-sec/microsdhc-security-32gb/dp/MD01443?st=uhs-i</v>
       </c>
     </row>
     <row r="11">
       <c r="D11" t="str">
-        <v>LED Ring</v>
+        <v>Okdo OV5647 Adjustable Focus</v>
       </c>
       <c r="E11" t="str">
-        <v>60mm 12V LED Ring for illumination</v>
+        <v>^^</v>
       </c>
       <c r="F11" t="str">
-        <v>3.40</v>
+        <v>9.83</v>
       </c>
       <c r="G11" t="str">
-        <v>https://www.aliexpress.com/item/4000212049737.html?spm=a2g0o.productlist.main.1.604b3ef99Jzoam&amp;algo_pvid=09ac1792-8ad0-47cc-b76e-9f8515ff91f3&amp;algo_exp_id=09ac1792-8ad0-47cc-b76e-9f8515ff91f3-0&amp;pdp_npi=4%40dis%21GBP%214.11%214.11%21%21%214.91%21%21%402103868d16995384407493038e472c%2110000001008603268%21sea%21UK%211802951889%21&amp;curPageLogUid=UuRZStryj55u</v>
+        <v>https://uk.rs-online.com/web/p/raspberry-pi-cameras/2020456</v>
+      </c>
+      <c r="H11" t="str">
+        <v>CAM</v>
+      </c>
+      <c r="I11" t="str">
+        <v>9.83</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="str">
-        <v>Power</v>
-      </c>
-      <c r="B12" t="str">
-        <v>PSU</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Power Supply Unit</v>
+      <c r="D12" t="str">
+        <v>IMX327LQR Adjustable Focus</v>
+      </c>
+      <c r="E12" t="str">
+        <v>^^</v>
+      </c>
+      <c r="F12" t="str">
+        <v>45</v>
+      </c>
+      <c r="H12" t="str">
+        <v>CAM</v>
       </c>
     </row>
     <row r="13">
+      <c r="C13" t="str">
+        <v/>
+      </c>
       <c r="D13" t="str">
-        <v>24V 150W Switching Power Supply</v>
+        <v>Ribbon Extension Cable</v>
       </c>
       <c r="E13" t="str">
-        <v xml:space="preserve">150W </v>
+        <v>300mm cable</v>
       </c>
       <c r="F13" t="str">
-        <v>20</v>
+        <v>1.20</v>
       </c>
       <c r="G13" t="str">
-        <v>https://uk.rs-online.com/web/p/switching-power-supplies/2411652?gb=s</v>
+        <v>https://onecall.farnell.com/pro-signal/ctlcamcableassy-300mm/cable-for-pi-camera-300mm-formed/dp/SC13282?st=camera%20ribbon</v>
+      </c>
+      <c r="I13" t="str">
+        <v>1.19</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" t="str">
-        <v>Cables</v>
-      </c>
-      <c r="C14" t="str">
-        <v>Connect Components</v>
-      </c>
       <c r="D14" t="str">
-        <v/>
+        <v>SD Card</v>
+      </c>
+      <c r="E14" t="str">
+        <v>32GB UHS-I U1 V10</v>
+      </c>
+      <c r="F14" t="str">
+        <v>8.30</v>
+      </c>
+      <c r="G14" t="str">
+        <v>https://onecall.farnell.com/integral/inmsdh32g10-sec/microsdhc-security-32gb/dp/MD01443?st=uhs-i</v>
+      </c>
+      <c r="I14" t="str">
+        <v>8.30</v>
       </c>
     </row>
     <row r="15">
       <c r="D15" t="str">
-        <v>18 awg</v>
+        <v>LED Ring</v>
       </c>
       <c r="E15" t="str">
-        <v>25m</v>
+        <v>60mm 12V LED Ring for illumination</v>
       </c>
       <c r="F15" t="str">
-        <v>10.27</v>
+        <v>3.40</v>
       </c>
       <c r="G15" t="str">
-        <v>https://uk.rs-online.com/web/p/hook-up-wire/8114422?gb=s</v>
+        <v>https://www.aliexpress.com/item/4000212049737.html?spm=a2g0o.productlist.main.1.604b3ef99Jzoam&amp;algo_pvid=09ac1792-8ad0-47cc-b76e-9f8515ff91f3&amp;algo_exp_id=09ac1792-8ad0-47cc-b76e-9f8515ff91f3-0&amp;pdp_npi=4%40dis%21GBP%214.11%214.11%21%21%214.91%21%21%402103868d16995384407493038e472c%2110000001008603268%21sea%21UK%211802951889%21&amp;curPageLogUid=UuRZStryj55u</v>
       </c>
     </row>
     <row r="16">
-      <c r="D16" t="str">
-        <v>Ribbon cables 28 awg</v>
-      </c>
-      <c r="E16" t="str">
-        <v>5m</v>
-      </c>
-      <c r="F16" t="str">
-        <v>4.82</v>
-      </c>
-      <c r="G16" t="str">
-        <v>https://onecall.farnell.com/pro-power/r2651dtsy10ac85/ribbon-cable-10-core-28awg-per/dp/2628358</v>
+      <c r="A16" t="str">
+        <v>Power</v>
+      </c>
+      <c r="B16" t="str">
+        <v>PSU</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Power Supply Unit</v>
       </c>
     </row>
     <row r="17">
       <c r="D17" t="str">
-        <v>JST Female Connectors</v>
+        <v>24V 150W Switching Power Supply</v>
       </c>
       <c r="E17" t="str">
-        <v>50pc</v>
+        <v xml:space="preserve">150W </v>
       </c>
       <c r="F17" t="str">
-        <v>4.70</v>
+        <v>20</v>
       </c>
       <c r="G17" t="str">
-        <v>https://uk.rs-online.com/web/p/circular-connector-contacts/6027900?gb=s</v>
+        <v>https://uk.rs-online.com/web/p/switching-power-supplies/2411652?gb=s</v>
+      </c>
+      <c r="I17" t="str">
+        <v>19.38</v>
       </c>
     </row>
     <row r="18">
+      <c r="B18" t="str">
+        <v>Cables</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Connect Components</v>
+      </c>
       <c r="D18" t="str">
-        <v>JST Male Connectors</v>
-      </c>
-      <c r="E18" t="str">
-        <v>100 pc</v>
-      </c>
-      <c r="F18" t="str">
-        <v>3.40</v>
-      </c>
-      <c r="G18" t="str">
-        <v>https://uk.rs-online.com/web/p/crimp-contacts/1613367?gb=s</v>
+        <v/>
       </c>
     </row>
     <row r="19">
-      <c r="B19" t="str">
-        <v>Transformers</v>
-      </c>
-      <c r="C19" t="str">
-        <v>Step down voltage</v>
+      <c r="D19" t="str">
+        <v>18 awg</v>
+      </c>
+      <c r="E19" t="str">
+        <v>25m</v>
+      </c>
+      <c r="F19" t="str">
+        <v>10.27</v>
+      </c>
+      <c r="G19" t="str">
+        <v>https://uk.rs-online.com/web/p/hook-up-wire/8114422?gb=s</v>
+      </c>
+      <c r="I19" t="str">
+        <v>10.24</v>
       </c>
     </row>
     <row r="20">
       <c r="D20" t="str">
+        <v>Ribbon cables 28 awg</v>
+      </c>
+      <c r="E20" t="str">
+        <v>6m</v>
+      </c>
+      <c r="F20" t="str">
+        <v>4.82</v>
+      </c>
+      <c r="G20" t="str">
+        <v>https://uk.farnell.com/pro-power/r2651dtsy10ac85/ribbon-cable-10-core-28awg-per/dp/2628358</v>
+      </c>
+      <c r="I20" t="str">
+        <v>4.82</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="D21" t="str">
+        <v>JST Female Connectors</v>
+      </c>
+      <c r="E21" t="str">
+        <v>50pc</v>
+      </c>
+      <c r="F21" t="str">
+        <v>4.70</v>
+      </c>
+      <c r="G21" t="str">
+        <v>https://uk.rs-online.com/web/p/circular-connector-contacts/6027900?gb=s</v>
+      </c>
+      <c r="I21" t="str">
+        <v>4.70</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="D22" t="str">
+        <v>JST Male Connectors</v>
+      </c>
+      <c r="E22" t="str">
+        <v>100 pc</v>
+      </c>
+      <c r="F22" t="str">
+        <v>3.40</v>
+      </c>
+      <c r="G22" t="str">
+        <v>https://uk.rs-online.com/web/p/crimp-contacts/1613367?gb=s</v>
+      </c>
+      <c r="I22" t="str">
+        <v>3.40</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" t="str">
+        <v>Heatshrink</v>
+      </c>
+      <c r="E23" t="str">
+        <v>150pc</v>
+      </c>
+      <c r="F23" t="str">
+        <v>8.45</v>
+      </c>
+      <c r="G23" t="str">
+        <v>https://uk.farnell.com/pro-power/pp3021/heatshrink-sleeving-kit-2-1-blk/dp/4161511?st=shrink%20tubing%20set</v>
+      </c>
+      <c r="I23" t="str">
+        <v>8.45</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="D24" t="str">
+        <v>Wire to board screw terminal single</v>
+      </c>
+      <c r="E24" t="str">
+        <v>20pc</v>
+      </c>
+      <c r="F24" t="str">
+        <v>8.12</v>
+      </c>
+      <c r="G24" t="str">
+        <v>https://uk.farnell.com/multicomp/mc000017/terminal-block-wire-to-brd-1pos/dp/2007984?st=screw%20terminal</v>
+      </c>
+      <c r="I24" t="str">
+        <v>8.12</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="D25" t="str">
+        <v>Wire stripper</v>
+      </c>
+      <c r="E25" t="str">
+        <v>1pc</v>
+      </c>
+      <c r="F25" t="str">
+        <v>2.15</v>
+      </c>
+      <c r="G25" t="str">
+        <v>https://uk.farnell.com/duratool/d03004/stripper-cutter-5-black-red/dp/2543007</v>
+      </c>
+      <c r="I25" t="str">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="D26" t="str">
+        <v>Ring terminal</v>
+      </c>
+      <c r="E26" t="str">
+        <v>20pc</v>
+      </c>
+      <c r="F26" t="str">
+        <v>3.38</v>
+      </c>
+      <c r="G26" t="str">
+        <v>https://uk.farnell.com/multicomp/crs-to-1806/terminal-ring-tongue-6-crimp/dp/1878197?st=wire%20to%20terminal%20connector</v>
+      </c>
+      <c r="I26" t="str">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="D27" t="str">
+        <v>Crimp tool 28awg-14awg</v>
+      </c>
+      <c r="E27" t="str">
+        <v>1pc</v>
+      </c>
+      <c r="F27" t="str">
+        <v>15.03</v>
+      </c>
+      <c r="G27" t="str">
+        <v>https://www.rapidonline.com/anvil-av-tct-5-way-terminal-crimping-tool-for-non-insulated-connectors-86-0521</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" t="str">
+        <v>Micro HDMI to HDMI</v>
+      </c>
+      <c r="E28" t="str">
+        <v>2m</v>
+      </c>
+      <c r="F28" t="str">
+        <v>5.56</v>
+      </c>
+      <c r="G28" t="str">
+        <v>https://uk.rs-online.com/web/p/hdmi-cables/1828766?gb=s</v>
+      </c>
+      <c r="I28" t="str">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="str">
+        <v>Transformers</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Step down voltage</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" t="str">
         <v>24V 5A Max</v>
       </c>
-      <c r="E20" t="str">
+      <c r="E30" t="str">
         <v>5 pc</v>
       </c>
-      <c r="F20" t="str">
+      <c r="F30" t="str">
         <v>9</v>
       </c>
-      <c r="G20" t="str">
+      <c r="G30" t="str">
         <v>https://www.aliexpress.com/item/1005006174030695.html?spm=a2g0o.productlist.main.1.5afa5fddD8qxg0&amp;algo_pvid=6e377741-5938-4c8d-bf97-6cff92cf4000&amp;algo_exp_id=6e377741-5938-4c8d-bf97-6cff92cf4000-0&amp;pdp_npi=4%40dis%21GBP%215.41%211.78%21%21%2146.97%21%21%402103835c16995438817356700ed5d4%2112000036120896530%21sea%21UK%211802951889%21&amp;curPageLogUid=pZiqGrlJTVoB</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="str">
+    <row r="31">
+      <c r="A31" t="str">
         <v>Screen</v>
       </c>
-      <c r="B21" t="str">
+      <c r="B31" t="str">
         <v>HDMI Screen</v>
       </c>
-      <c r="C21" t="str">
+      <c r="C31" t="str">
         <v>Display output using HDMI Connection</v>
       </c>
     </row>
-    <row r="23">
-      <c r="B23" t="str">
+    <row r="32">
+      <c r="D32" t="str">
+        <v>DFROBOT DFR0506</v>
+      </c>
+      <c r="E32" t="str">
+        <v>7 Inch</v>
+      </c>
+      <c r="F32" t="str">
+        <v>65</v>
+      </c>
+      <c r="G32" t="str">
+        <v>https://onecall.farnell.com/dfrobot/dfr0506/hdmi-display-embedded-dev-board/dp/3517851?st=hdmi%20screen</v>
+      </c>
+      <c r="I32" t="str">
+        <v>65.29</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="str">
         <v>GPIO TFT Screen</v>
       </c>
-      <c r="C23" t="str">
+      <c r="C33" t="str">
         <v>Output using GPIO</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Materials</v>
+      </c>
+      <c r="B34" t="str">
+        <v>PETG</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Prototyping</v>
+      </c>
+      <c r="D34" t="str">
+        <v>Solid Grey</v>
+      </c>
+      <c r="E34" t="str">
+        <v>1kg</v>
+      </c>
+      <c r="F34" t="str">
+        <v>19.80</v>
+      </c>
+      <c r="G34" t="str">
+        <v>https://3dfilaprint.com/product/esun-petg-solid-grey-1-75mm-1kg-3d-printing-filament/</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="D35" t="str">
+        <v>Solid Black</v>
+      </c>
+      <c r="E35" t="str">
+        <v>1kg</v>
+      </c>
+      <c r="F35" t="str">
+        <v>19.80</v>
+      </c>
+      <c r="G35" t="str">
+        <v>https://3dfilaprint.com/product/esun-petg-solid-black-1-75mm-1kg-3d-printing-filament/</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="str">
+        <v>Clear Plastic</v>
+      </c>
+      <c r="C36" t="str">
+        <v>For camera enclosure</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Clear</v>
+      </c>
+      <c r="E36" t="str">
+        <v>500x300x3mm</v>
+      </c>
+      <c r="F36" t="str">
+        <v>13.03</v>
+      </c>
+      <c r="G36" t="str">
+        <v>https://uk.rs-online.com/web/p/plastic-sheets/0434295?gb=s</v>
+      </c>
+      <c r="I36" t="str">
+        <v>13.03</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N23"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N36"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add to BOM and add camera test
</commit_message>
<xml_diff>
--- a/doc/BOM.xlsx
+++ b/doc/BOM.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,28 +416,40 @@
         <v>Component</v>
       </c>
       <c r="E1" t="str">
-        <v>Component Desc</v>
+        <v>Link</v>
       </c>
       <c r="F1" t="str">
         <v>Price</v>
       </c>
       <c r="G1" t="str">
-        <v>Link</v>
+        <v>Component Desc</v>
       </c>
       <c r="H1" t="str">
         <v>Dependencies</v>
       </c>
       <c r="I1" t="str">
-        <v>Bought?</v>
+        <v>Notes</v>
       </c>
       <c r="J1" t="str">
-        <v>Notes</v>
+        <v>Bought Batch 1</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Bought Batch 2</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Bought Batch 3</v>
       </c>
       <c r="M1" t="str">
-        <v>Total</v>
-      </c>
-      <c r="N1" t="str">
-        <v>=SUM(I2:i100)</v>
+        <v>Brought Myself</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Totals</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Batch 1:</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>=SUM(J2:J100)</v>
       </c>
     </row>
     <row r="2">
@@ -450,532 +462,691 @@
       <c r="C2" t="str">
         <v>Provides the system with real time computer vision capabilities</v>
       </c>
+      <c r="P2" t="str">
+        <v>Batch 2:</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>=SUM(K2:K100)</v>
+      </c>
     </row>
     <row r="3">
       <c r="D3" t="str">
         <v>Jetson Nano</v>
       </c>
       <c r="E3" t="str">
-        <v>Possesses GPU, GPIO pins and CSI camera interface, can control the entire project</v>
+        <v>https://uk.rs-online.com/web/p/processor-development-tools/1999831?gb=s</v>
       </c>
       <c r="F3" t="str">
         <v>134</v>
       </c>
       <c r="G3" t="str">
-        <v>https://uk.rs-online.com/web/p/processor-development-tools/1999831?gb=s</v>
-      </c>
-      <c r="I3" t="str">
+        <v>Possesses GPU, GPIO pins and CSI camera interface, can control the entire project</v>
+      </c>
+      <c r="J3" t="str">
         <v/>
       </c>
     </row>
+    <row r="4">
+      <c r="D4" t="str">
+        <v>Raspberry Pi 4B 4GB</v>
+      </c>
+      <c r="E4" t="str">
+        <v>https://onecall.farnell.com/raspberry-pi/rpi4-modbp-4gb/raspberry-pi-4-model-b-4gb/dp/3051887</v>
+      </c>
+      <c r="F4" t="str">
+        <v>45</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Raspberry Pi to handle the system, possess USB ports, GPIO, CSI Camera. May need a seperate GPU for inferencing</v>
+      </c>
+      <c r="H4" t="str">
+        <v>RPI</v>
+      </c>
+      <c r="I4" t="str">
+        <v>Got a 2GB model instead</v>
+      </c>
+      <c r="J4" t="str">
+        <v>45.46</v>
+      </c>
+      <c r="P4" t="str">
+        <v>Myself:</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>=SUM(M2:M100)</v>
+      </c>
+    </row>
     <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
       <c r="D5" t="str">
-        <v>Raspberry Pi 4B 4GB</v>
+        <v>Okdo ROCK 4 Model C+</v>
       </c>
       <c r="E5" t="str">
-        <v>Raspberry Pi to handle the system, possess USB ports, GPIO, CSI Camera. May need a seperate GPU for inferencing</v>
+        <v>https://uk.rs-online.com/web/p/rock-sbc-boards/2493158?intcmp=UK-WEB-_-CP-FP1-_-Dec-22-_-okdo-rock-single-4cplus</v>
       </c>
       <c r="F5" t="str">
         <v>45</v>
       </c>
       <c r="G5" t="str">
-        <v>https://onecall.farnell.com/raspberry-pi/rpi4-modbp-4gb/raspberry-pi-4-model-b-4gb/dp/3051887</v>
-      </c>
-      <c r="H5" t="str">
+        <v>RPi alternative with all the same inputs and outputs</v>
+      </c>
+      <c r="Q5" t="str">
+        <v>=SUM(Q1:Q5)</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="str">
+        <v>GPU Processor</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Seperate modules that provide AI inferencing capabilities</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" t="str">
+        <v>Intel Neural Compute Stick</v>
+      </c>
+      <c r="E7" t="str">
+        <v>https://uk.rs-online.com/web/p/processor-development-tools/1393655?gb=s</v>
+      </c>
+      <c r="F7" t="str">
+        <v>59</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Provides real time inferencing capabilties to the raspberry pi</v>
+      </c>
+      <c r="H7" t="str">
         <v>RPI</v>
       </c>
-      <c r="I5" t="str">
-        <v>45.46</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Vision</v>
+      </c>
+      <c r="B8" t="str">
+        <v>CSI Camera</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Camera used for the visionn system</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="str">
         <v/>
       </c>
-      <c r="D6" t="str">
-        <v>Okdo ROCK 4 Model C+</v>
-      </c>
-      <c r="E6" t="str">
-        <v>RPi alternative with all the same inputs and outputs</v>
-      </c>
-      <c r="F6" t="str">
-        <v>45</v>
-      </c>
-      <c r="G6" t="str">
-        <v>https://uk.rs-online.com/web/p/rock-sbc-boards/2493158?intcmp=UK-WEB-_-CP-FP1-_-Dec-22-_-okdo-rock-single-4cplus</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="str">
-        <v>GPU Processor</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Seperate modules that provide AI inferencing capabilities</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="D8" t="str">
-        <v>Intel Neural Compute Stick</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Provides real time inferencing capabilties to the raspberry pi</v>
-      </c>
-      <c r="F8" t="str">
-        <v>59</v>
-      </c>
-      <c r="G8" t="str">
-        <v>https://uk.rs-online.com/web/p/processor-development-tools/1393655?gb=s</v>
-      </c>
-      <c r="H8" t="str">
-        <v>RPI</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Vision</v>
-      </c>
-      <c r="B9" t="str">
-        <v>CSI Camera</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Camera used for the visionn system</v>
+      <c r="D9" t="str">
+        <v>OV5647 Camera Adjustable Focus</v>
+      </c>
+      <c r="E9" t="str">
+        <v>https://www.aliexpress.com/item/1005003386791483.html?spm=a2g0o.productlist.main.1.189a245aZHaLsB&amp;algo_pvid=260a6382-35b3-4d7e-86af-53e171ab5e10&amp;algo_exp_id=260a6382-35b3-4d7e-86af-53e171ab5e10-0&amp;pdp_npi=4%40dis%21GBP%215.45%215.45%21%21%216.50%21%21%40211b443e16995361090023304ee15b%2112000027225320432%21sea%21UK%211802951889%21&amp;curPageLogUid=gnYNy1UG26o0</v>
+      </c>
+      <c r="F9" t="str">
+        <v>6</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Adjustable focus camera, allows for macro shots</v>
+      </c>
+      <c r="H9" t="str">
+        <v>CAM</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Used here: https://www.instructables.com/RPi-MacroScope/</v>
       </c>
     </row>
     <row r="10">
-      <c r="C10" t="str">
-        <v/>
-      </c>
       <c r="D10" t="str">
-        <v>OV5647 Camera Adjustable Focus</v>
+        <v>Okdo OV5647 Adjustable Focus</v>
       </c>
       <c r="E10" t="str">
-        <v>Adjustable focus camera, allows for macro shots</v>
+        <v>https://uk.rs-online.com/web/p/raspberry-pi-cameras/2020456</v>
       </c>
       <c r="F10" t="str">
-        <v>6</v>
+        <v>9.83</v>
       </c>
       <c r="G10" t="str">
-        <v>https://www.aliexpress.com/item/1005003386791483.html?spm=a2g0o.productlist.main.1.189a245aZHaLsB&amp;algo_pvid=260a6382-35b3-4d7e-86af-53e171ab5e10&amp;algo_exp_id=260a6382-35b3-4d7e-86af-53e171ab5e10-0&amp;pdp_npi=4%40dis%21GBP%215.45%215.45%21%21%216.50%21%21%40211b443e16995361090023304ee15b%2112000027225320432%21sea%21UK%211802951889%21&amp;curPageLogUid=gnYNy1UG26o0</v>
+        <v>^^</v>
       </c>
       <c r="H10" t="str">
         <v>CAM</v>
       </c>
-      <c r="J10" t="str">
-        <v>Used here: https://www.instructables.com/RPi-MacroScope/</v>
-      </c>
     </row>
     <row r="11">
       <c r="D11" t="str">
-        <v>Okdo OV5647 Adjustable Focus</v>
-      </c>
-      <c r="E11" t="str">
+        <v>IMX327LQR Adjustable Focus</v>
+      </c>
+      <c r="F11" t="str">
+        <v>45</v>
+      </c>
+      <c r="G11" t="str">
         <v>^^</v>
-      </c>
-      <c r="F11" t="str">
-        <v>9.83</v>
-      </c>
-      <c r="G11" t="str">
-        <v>https://uk.rs-online.com/web/p/raspberry-pi-cameras/2020456</v>
       </c>
       <c r="H11" t="str">
         <v>CAM</v>
       </c>
-      <c r="I11" t="str">
-        <v>9.83</v>
-      </c>
     </row>
     <row r="12">
+      <c r="C12" t="str">
+        <v/>
+      </c>
       <c r="D12" t="str">
-        <v>IMX327LQR Adjustable Focus</v>
+        <v>Ribbon Extension Cable</v>
       </c>
       <c r="E12" t="str">
-        <v>^^</v>
+        <v>https://onecall.farnell.com/pro-signal/ctlcamcableassy-300mm/cable-for-pi-camera-300mm-formed/dp/SC13282?st=camera%20ribbon</v>
       </c>
       <c r="F12" t="str">
-        <v>45</v>
-      </c>
-      <c r="H12" t="str">
-        <v>CAM</v>
+        <v>1.20</v>
+      </c>
+      <c r="G12" t="str">
+        <v>300mm cable</v>
+      </c>
+      <c r="J12" t="str">
+        <v>1.19</v>
       </c>
     </row>
     <row r="13">
-      <c r="C13" t="str">
-        <v/>
-      </c>
       <c r="D13" t="str">
-        <v>Ribbon Extension Cable</v>
+        <v>SD Card</v>
       </c>
       <c r="E13" t="str">
-        <v>300mm cable</v>
+        <v>https://onecall.farnell.com/integral/inmsdh32g10-sec/microsdhc-security-32gb/dp/MD01443?st=uhs-i</v>
       </c>
       <c r="F13" t="str">
-        <v>1.20</v>
+        <v>8.30</v>
       </c>
       <c r="G13" t="str">
-        <v>https://onecall.farnell.com/pro-signal/ctlcamcableassy-300mm/cable-for-pi-camera-300mm-formed/dp/SC13282?st=camera%20ribbon</v>
-      </c>
-      <c r="I13" t="str">
-        <v>1.19</v>
+        <v>32GB UHS-I U1 V10</v>
+      </c>
+      <c r="J13" t="str">
+        <v>8.30</v>
       </c>
     </row>
     <row r="14">
       <c r="D14" t="str">
-        <v>SD Card</v>
+        <v>LED Ring</v>
       </c>
       <c r="E14" t="str">
-        <v>32GB UHS-I U1 V10</v>
+        <v>https://www.aliexpress.com/item/4000212049737.html?spm=a2g0o.productlist.main.1.604b3ef99Jzoam&amp;algo_pvid=09ac1792-8ad0-47cc-b76e-9f8515ff91f3&amp;algo_exp_id=09ac1792-8ad0-47cc-b76e-9f8515ff91f3-0&amp;pdp_npi=4%40dis%21GBP%214.11%214.11%21%21%214.91%21%21%402103868d16995384407493038e472c%2110000001008603268%21sea%21UK%211802951889%21&amp;curPageLogUid=UuRZStryj55u</v>
       </c>
       <c r="F14" t="str">
-        <v>8.30</v>
+        <v>3.40</v>
       </c>
       <c r="G14" t="str">
-        <v>https://onecall.farnell.com/integral/inmsdh32g10-sec/microsdhc-security-32gb/dp/MD01443?st=uhs-i</v>
-      </c>
-      <c r="I14" t="str">
-        <v>8.30</v>
+        <v>80mm 12V LED Ring for illumination 2pc</v>
       </c>
     </row>
     <row r="15">
-      <c r="D15" t="str">
-        <v>LED Ring</v>
-      </c>
-      <c r="E15" t="str">
-        <v>60mm 12V LED Ring for illumination</v>
-      </c>
-      <c r="F15" t="str">
-        <v>3.40</v>
-      </c>
-      <c r="G15" t="str">
-        <v>https://www.aliexpress.com/item/4000212049737.html?spm=a2g0o.productlist.main.1.604b3ef99Jzoam&amp;algo_pvid=09ac1792-8ad0-47cc-b76e-9f8515ff91f3&amp;algo_exp_id=09ac1792-8ad0-47cc-b76e-9f8515ff91f3-0&amp;pdp_npi=4%40dis%21GBP%214.11%214.11%21%21%214.91%21%21%402103868d16995384407493038e472c%2110000001008603268%21sea%21UK%211802951889%21&amp;curPageLogUid=UuRZStryj55u</v>
+      <c r="A15" t="str">
+        <v>Components</v>
+      </c>
+      <c r="B15" t="str">
+        <v>PSU</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Power Supply Unit</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="str">
-        <v>Power</v>
-      </c>
-      <c r="B16" t="str">
-        <v>PSU</v>
-      </c>
-      <c r="C16" t="str">
-        <v>Power Supply Unit</v>
+      <c r="D16" t="str">
+        <v>24V 150W Switching Power Supply</v>
+      </c>
+      <c r="E16" t="str">
+        <v>https://uk.rs-online.com/web/p/switching-power-supplies/2411652?gb=s</v>
+      </c>
+      <c r="F16" t="str">
+        <v>20</v>
+      </c>
+      <c r="G16" t="str">
+        <v xml:space="preserve">150W </v>
+      </c>
+      <c r="J16" t="str">
+        <v>19.38</v>
       </c>
     </row>
     <row r="17">
+      <c r="B17" t="str">
+        <v>Cables</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Connect Components</v>
+      </c>
       <c r="D17" t="str">
-        <v>24V 150W Switching Power Supply</v>
-      </c>
-      <c r="E17" t="str">
-        <v xml:space="preserve">150W </v>
-      </c>
-      <c r="F17" t="str">
-        <v>20</v>
-      </c>
-      <c r="G17" t="str">
-        <v>https://uk.rs-online.com/web/p/switching-power-supplies/2411652?gb=s</v>
-      </c>
-      <c r="I17" t="str">
-        <v>19.38</v>
+        <v/>
       </c>
     </row>
     <row r="18">
-      <c r="B18" t="str">
-        <v>Cables</v>
-      </c>
-      <c r="C18" t="str">
-        <v>Connect Components</v>
-      </c>
       <c r="D18" t="str">
-        <v/>
+        <v>4 Way USB Hub</v>
+      </c>
+      <c r="E18" t="str">
+        <v>https://onecall.farnell.com/dynamode/usb3-hb-4pm-v2/hub-4-port-usb-a-to-4-x-usb-a/dp/CS35947</v>
+      </c>
+      <c r="F18" t="str">
+        <v>8.99</v>
+      </c>
+      <c r="G18" t="str">
+        <v>3pc</v>
+      </c>
+      <c r="K18" t="str">
+        <v>8.99</v>
       </c>
     </row>
     <row r="19">
       <c r="D19" t="str">
-        <v>18 awg</v>
+        <v>USB A to USB C 3pc</v>
       </c>
       <c r="E19" t="str">
-        <v>25m</v>
+        <v>https://onecall.farnell.com/newlink/nlmob-941bdbk/lead-usb2-0-a-c-m-m-black-braided/dp/CS35766?st=usb%20c%20cable</v>
       </c>
       <c r="F19" t="str">
-        <v>10.27</v>
+        <v>6.42</v>
       </c>
       <c r="G19" t="str">
-        <v>https://uk.rs-online.com/web/p/hook-up-wire/8114422?gb=s</v>
-      </c>
-      <c r="I19" t="str">
-        <v>10.24</v>
+        <v>3pc</v>
+      </c>
+      <c r="K19" t="str">
+        <v>6.42</v>
       </c>
     </row>
     <row r="20">
       <c r="D20" t="str">
-        <v>Ribbon cables 28 awg</v>
+        <v>USB A to Micro B 3pc</v>
       </c>
       <c r="E20" t="str">
-        <v>6m</v>
+        <v>https://onecall.farnell.com/pro-signal/psg91471/lead-usb2-0-a-male-micro-b-male/dp/3498532?st=micro%20usb%20cable</v>
       </c>
       <c r="F20" t="str">
-        <v>4.82</v>
+        <v>5.94</v>
       </c>
       <c r="G20" t="str">
-        <v>https://uk.farnell.com/pro-power/r2651dtsy10ac85/ribbon-cable-10-core-28awg-per/dp/2628358</v>
-      </c>
-      <c r="I20" t="str">
-        <v>4.82</v>
+        <v>3pc</v>
+      </c>
+      <c r="K20" t="str">
+        <v>5.94</v>
       </c>
     </row>
     <row r="21">
       <c r="D21" t="str">
-        <v>JST Female Connectors</v>
+        <v>USB C to C</v>
       </c>
       <c r="E21" t="str">
-        <v>50pc</v>
+        <v>https://onecall.farnell.com/pro-signal/psg91210/lead-usb2-0-type-c-type-c-1m-black/dp/CS28720?st=usb%20c%20to%20usb%20c</v>
       </c>
       <c r="F21" t="str">
-        <v>4.70</v>
+        <v>3.61</v>
       </c>
       <c r="G21" t="str">
-        <v>https://uk.rs-online.com/web/p/circular-connector-contacts/6027900?gb=s</v>
-      </c>
-      <c r="I21" t="str">
-        <v>4.70</v>
+        <v>1pc</v>
+      </c>
+      <c r="K21" t="str">
+        <v>3.61</v>
       </c>
     </row>
     <row r="22">
       <c r="D22" t="str">
-        <v>JST Male Connectors</v>
+        <v>18 awg</v>
       </c>
       <c r="E22" t="str">
-        <v>100 pc</v>
+        <v>https://uk.rs-online.com/web/p/hook-up-wire/8114422?gb=s</v>
       </c>
       <c r="F22" t="str">
-        <v>3.40</v>
+        <v>10.27</v>
       </c>
       <c r="G22" t="str">
-        <v>https://uk.rs-online.com/web/p/crimp-contacts/1613367?gb=s</v>
-      </c>
-      <c r="I22" t="str">
-        <v>3.40</v>
+        <v>25m</v>
+      </c>
+      <c r="J22" t="str">
+        <v>10.24</v>
       </c>
     </row>
     <row r="23">
       <c r="D23" t="str">
-        <v>Heatshrink</v>
+        <v>Ribbon cables 28 awg</v>
       </c>
       <c r="E23" t="str">
-        <v>150pc</v>
+        <v>https://uk.farnell.com/pro-power/r2651dtsy10ac85/ribbon-cable-10-core-28awg-per/dp/2628358</v>
       </c>
       <c r="F23" t="str">
-        <v>8.45</v>
+        <v>4.82</v>
       </c>
       <c r="G23" t="str">
-        <v>https://uk.farnell.com/pro-power/pp3021/heatshrink-sleeving-kit-2-1-blk/dp/4161511?st=shrink%20tubing%20set</v>
-      </c>
-      <c r="I23" t="str">
-        <v>8.45</v>
+        <v>6m</v>
+      </c>
+      <c r="K23" t="str">
+        <v>4.82</v>
       </c>
     </row>
     <row r="24">
       <c r="D24" t="str">
-        <v>Wire to board screw terminal single</v>
+        <v>Wire stripper</v>
       </c>
       <c r="E24" t="str">
-        <v>20pc</v>
+        <v>https://uk.farnell.com/duratool/d03004/stripper-cutter-5-black-red/dp/2543007</v>
       </c>
       <c r="F24" t="str">
-        <v>8.12</v>
+        <v>2.15</v>
       </c>
       <c r="G24" t="str">
-        <v>https://uk.farnell.com/multicomp/mc000017/terminal-block-wire-to-brd-1pos/dp/2007984?st=screw%20terminal</v>
-      </c>
-      <c r="I24" t="str">
-        <v>8.12</v>
+        <v>1pc</v>
+      </c>
+      <c r="J24" t="str">
+        <v>2.15</v>
       </c>
     </row>
     <row r="25">
       <c r="D25" t="str">
-        <v>Wire stripper</v>
+        <v>Micro HDMI to HDMI</v>
       </c>
       <c r="E25" t="str">
-        <v>1pc</v>
+        <v>https://uk.rs-online.com/web/p/hdmi-cables/1828766?gb=s</v>
       </c>
       <c r="F25" t="str">
-        <v>2.15</v>
+        <v>5.56</v>
       </c>
       <c r="G25" t="str">
-        <v>https://uk.farnell.com/duratool/d03004/stripper-cutter-5-black-red/dp/2543007</v>
-      </c>
-      <c r="I25" t="str">
-        <v>2.15</v>
+        <v>2m</v>
+      </c>
+      <c r="J25" t="str">
+        <v>5.56</v>
       </c>
     </row>
     <row r="26">
       <c r="D26" t="str">
-        <v>Ring terminal</v>
+        <v>Heatshrink</v>
       </c>
       <c r="E26" t="str">
-        <v>20pc</v>
+        <v>https://uk.farnell.com/pro-power/pp3021/heatshrink-sleeving-kit-2-1-blk/dp/4161511?st=shrink%20tubing%20set</v>
       </c>
       <c r="F26" t="str">
-        <v>3.38</v>
+        <v>8.45</v>
       </c>
       <c r="G26" t="str">
-        <v>https://uk.farnell.com/multicomp/crs-to-1806/terminal-ring-tongue-6-crimp/dp/1878197?st=wire%20to%20terminal%20connector</v>
-      </c>
-      <c r="I26" t="str">
-        <v>3.38</v>
+        <v>150pc</v>
+      </c>
+      <c r="J26" t="str">
+        <v>8.45</v>
       </c>
     </row>
     <row r="27">
-      <c r="D27" t="str">
-        <v>Crimp tool 28awg-14awg</v>
-      </c>
-      <c r="E27" t="str">
-        <v>1pc</v>
-      </c>
-      <c r="F27" t="str">
-        <v>15.03</v>
-      </c>
-      <c r="G27" t="str">
-        <v>https://www.rapidonline.com/anvil-av-tct-5-way-terminal-crimping-tool-for-non-insulated-connectors-86-0521</v>
+      <c r="B27" t="str">
+        <v>Boards</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Allow prototyping by placing components on a board</v>
       </c>
     </row>
     <row r="28">
       <c r="D28" t="str">
-        <v>Micro HDMI to HDMI</v>
+        <v>150 Point Through Hole</v>
       </c>
       <c r="E28" t="str">
-        <v>2m</v>
+        <v>https://onecall.farnell.com/proto-advantage/sbbth1510-1/solder-breadboard-150-holes/dp/PC02483</v>
       </c>
       <c r="F28" t="str">
-        <v>5.56</v>
+        <v>5.97</v>
       </c>
       <c r="G28" t="str">
-        <v>https://uk.rs-online.com/web/p/hdmi-cables/1828766?gb=s</v>
-      </c>
-      <c r="I28" t="str">
-        <v>5.56</v>
+        <v>3pc</v>
+      </c>
+      <c r="K28" t="str">
+        <v>5.97</v>
       </c>
     </row>
     <row r="29">
-      <c r="B29" t="str">
-        <v>Transformers</v>
-      </c>
-      <c r="C29" t="str">
-        <v>Step down voltage</v>
+      <c r="D29" t="str">
+        <v>Breadboard Small</v>
+      </c>
+      <c r="E29" t="str">
+        <v>https://onecall.farnell.com/cyntech/breadboard170red/breadboard-mini-red/dp/PC01594</v>
+      </c>
+      <c r="F29" t="str">
+        <v>4.11</v>
+      </c>
+      <c r="G29" t="str">
+        <v>3pc</v>
+      </c>
+      <c r="K29" t="str">
+        <v>4.11</v>
       </c>
     </row>
     <row r="30">
-      <c r="D30" t="str">
-        <v>24V 5A Max</v>
-      </c>
-      <c r="E30" t="str">
-        <v>5 pc</v>
-      </c>
-      <c r="F30" t="str">
-        <v>9</v>
-      </c>
-      <c r="G30" t="str">
-        <v>https://www.aliexpress.com/item/1005006174030695.html?spm=a2g0o.productlist.main.1.5afa5fddD8qxg0&amp;algo_pvid=6e377741-5938-4c8d-bf97-6cff92cf4000&amp;algo_exp_id=6e377741-5938-4c8d-bf97-6cff92cf4000-0&amp;pdp_npi=4%40dis%21GBP%215.41%211.78%21%21%2146.97%21%21%402103835c16995438817356700ed5d4%2112000036120896530%21sea%21UK%211802951889%21&amp;curPageLogUid=pZiqGrlJTVoB</v>
+      <c r="B30" t="str">
+        <v>Connectors</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Connect wires or components to each other</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="str">
-        <v>Screen</v>
-      </c>
-      <c r="B31" t="str">
-        <v>HDMI Screen</v>
-      </c>
-      <c r="C31" t="str">
-        <v>Display output using HDMI Connection</v>
+      <c r="D31" t="str">
+        <v>Ring terminal</v>
+      </c>
+      <c r="E31" t="str">
+        <v>https://uk.farnell.com/multicomp/crs-to-1806/terminal-ring-tongue-6-crimp/dp/1878197?st=wire%20to%20terminal%20connector</v>
+      </c>
+      <c r="F31" t="str">
+        <v>3.38</v>
+      </c>
+      <c r="G31" t="str">
+        <v>20pc</v>
+      </c>
+      <c r="J31" t="str">
+        <v>3.38</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="str">
-        <v>DFROBOT DFR0506</v>
+        <v>JST Female Connectors</v>
       </c>
       <c r="E32" t="str">
-        <v>7 Inch</v>
+        <v>https://uk.rs-online.com/web/p/circular-connector-contacts/6027900?gb=s</v>
       </c>
       <c r="F32" t="str">
-        <v>65</v>
+        <v>4.70</v>
       </c>
       <c r="G32" t="str">
-        <v>https://onecall.farnell.com/dfrobot/dfr0506/hdmi-display-embedded-dev-board/dp/3517851?st=hdmi%20screen</v>
-      </c>
-      <c r="I32" t="str">
-        <v>65.29</v>
+        <v>50pc</v>
+      </c>
+      <c r="J32" t="str">
+        <v>4.70</v>
       </c>
     </row>
     <row r="33">
-      <c r="B33" t="str">
-        <v>GPIO TFT Screen</v>
-      </c>
-      <c r="C33" t="str">
-        <v>Output using GPIO</v>
+      <c r="D33" t="str">
+        <v>JST Male Connectors</v>
+      </c>
+      <c r="E33" t="str">
+        <v>https://uk.rs-online.com/web/p/crimp-contacts/1613367?gb=s</v>
+      </c>
+      <c r="F33" t="str">
+        <v>3.40</v>
+      </c>
+      <c r="G33" t="str">
+        <v>100pc</v>
+      </c>
+      <c r="J33" t="str">
+        <v>3.40</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="str">
-        <v>Materials</v>
-      </c>
-      <c r="B34" t="str">
-        <v>PETG</v>
-      </c>
-      <c r="C34" t="str">
-        <v>Prototyping</v>
-      </c>
       <c r="D34" t="str">
-        <v>Solid Grey</v>
+        <v>Wire to board screw terminal single</v>
       </c>
       <c r="E34" t="str">
-        <v>1kg</v>
+        <v>https://uk.farnell.com/multicomp/mc000017/terminal-block-wire-to-brd-1pos/dp/2007984?st=screw%20terminal</v>
       </c>
       <c r="F34" t="str">
-        <v>19.80</v>
+        <v>8.12</v>
       </c>
       <c r="G34" t="str">
-        <v>https://3dfilaprint.com/product/esun-petg-solid-grey-1-75mm-1kg-3d-printing-filament/</v>
+        <v>20pc</v>
+      </c>
+      <c r="J34" t="str">
+        <v>8.12</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="str">
-        <v>Solid Black</v>
+        <v>USB Female Breakout</v>
       </c>
       <c r="E35" t="str">
-        <v>1kg</v>
+        <v>https://onecall.farnell.com/clever-little-box/cie-yy24/usb-2-0-a-socket-breakout-board/dp/CN22556</v>
       </c>
       <c r="F35" t="str">
-        <v>19.80</v>
+        <v>5.10</v>
       </c>
       <c r="G35" t="str">
-        <v>https://3dfilaprint.com/product/esun-petg-solid-black-1-75mm-1kg-3d-printing-filament/</v>
+        <v>5pc</v>
+      </c>
+      <c r="K35" t="str">
+        <v>5.10</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="str">
+        <v>Electronics</v>
+      </c>
+      <c r="C36" t="str">
+        <v>IRF520N</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="D37" t="str">
+        <v>N Channel Mosfet to allow the Pi to control high voltage or high current components</v>
+      </c>
+      <c r="E37" t="str">
+        <v>https://onecall.farnell.com/vishay/irf520pbf/mosfet-n-100v-9-2a-to-220/dp/8648239?st=irf520</v>
+      </c>
+      <c r="F37" t="str">
+        <v>6.10</v>
+      </c>
+      <c r="G37" t="str">
+        <v>5pc</v>
+      </c>
+      <c r="K37" t="str">
+        <v>6.10</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="str">
+        <v>Transformers</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Step down voltage</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" t="str">
+        <v>24V 5A Max</v>
+      </c>
+      <c r="E39" t="str">
+        <v>https://www.aliexpress.com/item/1005006174030695.html?spm=a2g0o.productlist.main.1.5afa5fddD8qxg0&amp;algo_pvid=6e377741-5938-4c8d-bf97-6cff92cf4000&amp;algo_exp_id=6e377741-5938-4c8d-bf97-6cff92cf4000-0&amp;pdp_npi=4%40dis%21GBP%215.41%211.78%21%21%2146.97%21%21%402103835c16995438817356700ed5d4%2112000036120896530%21sea%21UK%211802951889%21&amp;curPageLogUid=pZiqGrlJTVoB</v>
+      </c>
+      <c r="F39" t="str">
+        <v>9</v>
+      </c>
+      <c r="G39" t="str">
+        <v>5 pc</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Screen</v>
+      </c>
+      <c r="B40" t="str">
+        <v>HDMI Screen</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Display output using HDMI Connection</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" t="str">
+        <v>DFROBOT DFR0506</v>
+      </c>
+      <c r="E41" t="str">
+        <v>https://onecall.farnell.com/dfrobot/dfr0506/hdmi-display-embedded-dev-board/dp/3517851?st=hdmi%20screen</v>
+      </c>
+      <c r="F41" t="str">
+        <v>65</v>
+      </c>
+      <c r="G41" t="str">
+        <v>7 Inch</v>
+      </c>
+      <c r="J41" t="str">
+        <v>65.29</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Materials</v>
+      </c>
+      <c r="B42" t="str">
+        <v>PETG</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Prototyping</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Solid Grey</v>
+      </c>
+      <c r="E42" t="str">
+        <v>https://3dfilaprint.com/product/esun-petg-solid-grey-1-75mm-1kg-3d-printing-filament/</v>
+      </c>
+      <c r="F42" t="str">
+        <v>16</v>
+      </c>
+      <c r="G42" t="str">
+        <v>1kg</v>
+      </c>
+      <c r="J42" t="str">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="D43" t="str">
+        <v>Solid Black</v>
+      </c>
+      <c r="E43" t="str">
+        <v>https://3dfilaprint.com/product/esun-petg-solid-black-1-75mm-1kg-3d-printing-filament/</v>
+      </c>
+      <c r="F43" t="str">
+        <v>16</v>
+      </c>
+      <c r="G43" t="str">
+        <v>1kg</v>
+      </c>
+      <c r="J43" t="str">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="str">
         <v>Clear Plastic</v>
       </c>
-      <c r="C36" t="str">
+      <c r="C44" t="str">
         <v>For camera enclosure</v>
       </c>
-      <c r="D36" t="str">
+      <c r="D44" t="str">
         <v>Clear</v>
       </c>
-      <c r="E36" t="str">
+      <c r="E44" t="str">
+        <v>https://uk.rs-online.com/web/p/plastic-sheets/0434295?gb=s</v>
+      </c>
+      <c r="F44" t="str">
+        <v>13.03</v>
+      </c>
+      <c r="G44" t="str">
         <v>500x300x3mm</v>
       </c>
-      <c r="F36" t="str">
-        <v>13.03</v>
-      </c>
-      <c r="G36" t="str">
-        <v>https://uk.rs-online.com/web/p/plastic-sheets/0434295?gb=s</v>
-      </c>
-      <c r="I36" t="str">
+      <c r="J44" t="str">
         <v>13.03</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N36"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q44"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more to BOM, increase camera cover height
</commit_message>
<xml_diff>
--- a/doc/BOM.xlsx
+++ b/doc/BOM.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q44"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -610,6 +610,9 @@
       <c r="H10" t="str">
         <v>CAM</v>
       </c>
+      <c r="J10" t="str">
+        <v>9.83</v>
+      </c>
     </row>
     <row r="11">
       <c r="D11" t="str">
@@ -644,6 +647,9 @@
       <c r="J12" t="str">
         <v>1.19</v>
       </c>
+      <c r="M12" t="str">
+        <v>2.20</v>
+      </c>
     </row>
     <row r="13">
       <c r="D13" t="str">
@@ -675,6 +681,9 @@
       <c r="G14" t="str">
         <v>80mm 12V LED Ring for illumination 2pc</v>
       </c>
+      <c r="M14" t="str">
+        <v>6.00</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -705,448 +714,516 @@
       </c>
     </row>
     <row r="17">
-      <c r="B17" t="str">
-        <v>Cables</v>
-      </c>
-      <c r="C17" t="str">
-        <v>Connect Components</v>
-      </c>
       <c r="D17" t="str">
-        <v/>
+        <v>C14 IEC20 Connector</v>
+      </c>
+      <c r="E17" t="str">
+        <v>https://uk.rs-online.com/web/p/iec-connectors/8117216</v>
+      </c>
+      <c r="F17" t="str">
+        <v>3.71</v>
+      </c>
+      <c r="G17" t="str">
+        <v>2pc</v>
+      </c>
+      <c r="K17" t="str">
+        <v>7.42</v>
       </c>
     </row>
     <row r="18">
       <c r="D18" t="str">
-        <v>4 Way USB Hub</v>
+        <v>IEC C13 Socket to Type G UK Plug</v>
       </c>
       <c r="E18" t="str">
-        <v>https://onecall.farnell.com/dynamode/usb3-hb-4pm-v2/hub-4-port-usb-a-to-4-x-usb-a/dp/CS35947</v>
+        <v>https://uk.rs-online.com/web/p/power-cords/1469109?gb=s</v>
       </c>
       <c r="F18" t="str">
-        <v>8.99</v>
+        <v>4.46</v>
       </c>
       <c r="G18" t="str">
-        <v>3pc</v>
+        <v>1.8m</v>
       </c>
       <c r="K18" t="str">
-        <v>8.99</v>
+        <v>4.46</v>
       </c>
     </row>
     <row r="19">
       <c r="D19" t="str">
-        <v>USB A to USB C 3pc</v>
+        <v>6A T Glass Cartridge Fuse, 5 x 20mm</v>
       </c>
       <c r="E19" t="str">
-        <v>https://onecall.farnell.com/newlink/nlmob-941bdbk/lead-usb2-0-a-c-m-m-black-braided/dp/CS35766?st=usb%20c%20cable</v>
+        <v>https://uk.rs-online.com/web/p/cartridge-fuses/9113427?gb=s</v>
       </c>
       <c r="F19" t="str">
-        <v>6.42</v>
+        <v>0.333</v>
       </c>
       <c r="G19" t="str">
-        <v>3pc</v>
+        <v>10pc</v>
       </c>
       <c r="K19" t="str">
-        <v>6.42</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="20">
+      <c r="B20" t="str">
+        <v>Cables</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Connect Components</v>
+      </c>
       <c r="D20" t="str">
-        <v>USB A to Micro B 3pc</v>
-      </c>
-      <c r="E20" t="str">
-        <v>https://onecall.farnell.com/pro-signal/psg91471/lead-usb2-0-a-male-micro-b-male/dp/3498532?st=micro%20usb%20cable</v>
-      </c>
-      <c r="F20" t="str">
-        <v>5.94</v>
-      </c>
-      <c r="G20" t="str">
-        <v>3pc</v>
-      </c>
-      <c r="K20" t="str">
-        <v>5.94</v>
+        <v/>
       </c>
     </row>
     <row r="21">
       <c r="D21" t="str">
-        <v>USB C to C</v>
+        <v>4 Way USB Hub</v>
       </c>
       <c r="E21" t="str">
-        <v>https://onecall.farnell.com/pro-signal/psg91210/lead-usb2-0-type-c-type-c-1m-black/dp/CS28720?st=usb%20c%20to%20usb%20c</v>
+        <v>https://onecall.farnell.com/dynamode/usb3-hb-4pm-v2/hub-4-port-usb-a-to-4-x-usb-a/dp/CS35947</v>
       </c>
       <c r="F21" t="str">
-        <v>3.61</v>
+        <v>8.99</v>
       </c>
       <c r="G21" t="str">
-        <v>1pc</v>
+        <v>3pc</v>
       </c>
       <c r="K21" t="str">
-        <v>3.61</v>
+        <v>8.99</v>
       </c>
     </row>
     <row r="22">
       <c r="D22" t="str">
-        <v>18 awg</v>
+        <v>USB A to USB C 3pc</v>
       </c>
       <c r="E22" t="str">
-        <v>https://uk.rs-online.com/web/p/hook-up-wire/8114422?gb=s</v>
+        <v>https://onecall.farnell.com/newlink/nlmob-941bdbk/lead-usb2-0-a-c-m-m-black-braided/dp/CS35766?st=usb%20c%20cable</v>
       </c>
       <c r="F22" t="str">
-        <v>10.27</v>
+        <v>6.42</v>
       </c>
       <c r="G22" t="str">
-        <v>25m</v>
-      </c>
-      <c r="J22" t="str">
-        <v>10.24</v>
+        <v>3pc</v>
+      </c>
+      <c r="K22" t="str">
+        <v>6.42</v>
       </c>
     </row>
     <row r="23">
       <c r="D23" t="str">
-        <v>Ribbon cables 28 awg</v>
+        <v>USB A to Micro B 3pc</v>
       </c>
       <c r="E23" t="str">
-        <v>https://uk.farnell.com/pro-power/r2651dtsy10ac85/ribbon-cable-10-core-28awg-per/dp/2628358</v>
+        <v>https://onecall.farnell.com/pro-signal/psg91471/lead-usb2-0-a-male-micro-b-male/dp/3498532?st=micro%20usb%20cable</v>
       </c>
       <c r="F23" t="str">
-        <v>4.82</v>
+        <v>5.94</v>
       </c>
       <c r="G23" t="str">
-        <v>6m</v>
+        <v>3pc</v>
       </c>
       <c r="K23" t="str">
-        <v>4.82</v>
+        <v>5.94</v>
       </c>
     </row>
     <row r="24">
       <c r="D24" t="str">
-        <v>Wire stripper</v>
+        <v>USB C to C</v>
       </c>
       <c r="E24" t="str">
-        <v>https://uk.farnell.com/duratool/d03004/stripper-cutter-5-black-red/dp/2543007</v>
+        <v>https://onecall.farnell.com/pro-signal/psg91210/lead-usb2-0-type-c-type-c-1m-black/dp/CS28720?st=usb%20c%20to%20usb%20c</v>
       </c>
       <c r="F24" t="str">
-        <v>2.15</v>
+        <v>3.61</v>
       </c>
       <c r="G24" t="str">
         <v>1pc</v>
       </c>
-      <c r="J24" t="str">
-        <v>2.15</v>
+      <c r="K24" t="str">
+        <v>3.61</v>
       </c>
     </row>
     <row r="25">
       <c r="D25" t="str">
-        <v>Micro HDMI to HDMI</v>
+        <v>18 awg red</v>
       </c>
       <c r="E25" t="str">
-        <v>https://uk.rs-online.com/web/p/hdmi-cables/1828766?gb=s</v>
+        <v>https://uk.rs-online.com/web/p/hook-up-wire/8114422?gb=s</v>
       </c>
       <c r="F25" t="str">
-        <v>5.56</v>
+        <v>10.27</v>
       </c>
       <c r="G25" t="str">
-        <v>2m</v>
+        <v>25m</v>
       </c>
       <c r="J25" t="str">
-        <v>5.56</v>
+        <v>10.27</v>
       </c>
     </row>
     <row r="26">
       <c r="D26" t="str">
-        <v>Heatshrink</v>
+        <v>18 awg black</v>
       </c>
       <c r="E26" t="str">
-        <v>https://uk.farnell.com/pro-power/pp3021/heatshrink-sleeving-kit-2-1-blk/dp/4161511?st=shrink%20tubing%20set</v>
+        <v>https://uk.rs-online.com/web/p/hook-up-wire/8114416?gb=s</v>
       </c>
       <c r="F26" t="str">
-        <v>8.45</v>
+        <v>10.27</v>
       </c>
       <c r="G26" t="str">
-        <v>150pc</v>
-      </c>
-      <c r="J26" t="str">
-        <v>8.45</v>
+        <v>25m</v>
+      </c>
+      <c r="K26" t="str">
+        <v>10.27</v>
       </c>
     </row>
     <row r="27">
-      <c r="B27" t="str">
-        <v>Boards</v>
-      </c>
-      <c r="C27" t="str">
-        <v>Allow prototyping by placing components on a board</v>
+      <c r="D27" t="str">
+        <v>Ribbon cables 28 awg</v>
+      </c>
+      <c r="E27" t="str">
+        <v>https://uk.farnell.com/pro-power/r2651dtsy10ac85/ribbon-cable-10-core-28awg-per/dp/2628358</v>
+      </c>
+      <c r="F27" t="str">
+        <v>4.82</v>
+      </c>
+      <c r="G27" t="str">
+        <v>6m</v>
+      </c>
+      <c r="K27" t="str">
+        <v>4.82</v>
       </c>
     </row>
     <row r="28">
       <c r="D28" t="str">
-        <v>150 Point Through Hole</v>
+        <v>Wire stripper</v>
       </c>
       <c r="E28" t="str">
-        <v>https://onecall.farnell.com/proto-advantage/sbbth1510-1/solder-breadboard-150-holes/dp/PC02483</v>
+        <v>https://uk.farnell.com/duratool/d03004/stripper-cutter-5-black-red/dp/2543007</v>
       </c>
       <c r="F28" t="str">
-        <v>5.97</v>
+        <v>2.15</v>
       </c>
       <c r="G28" t="str">
-        <v>3pc</v>
-      </c>
-      <c r="K28" t="str">
-        <v>5.97</v>
+        <v>1pc</v>
+      </c>
+      <c r="J28" t="str">
+        <v>2.15</v>
       </c>
     </row>
     <row r="29">
       <c r="D29" t="str">
-        <v>Breadboard Small</v>
+        <v>Micro HDMI to HDMI</v>
       </c>
       <c r="E29" t="str">
-        <v>https://onecall.farnell.com/cyntech/breadboard170red/breadboard-mini-red/dp/PC01594</v>
+        <v>https://uk.rs-online.com/web/p/hdmi-cables/1828766?gb=s</v>
       </c>
       <c r="F29" t="str">
-        <v>4.11</v>
+        <v>5.56</v>
       </c>
       <c r="G29" t="str">
-        <v>3pc</v>
-      </c>
-      <c r="K29" t="str">
-        <v>4.11</v>
+        <v>2m</v>
+      </c>
+      <c r="J29" t="str">
+        <v>5.56</v>
       </c>
     </row>
     <row r="30">
-      <c r="B30" t="str">
-        <v>Connectors</v>
-      </c>
-      <c r="C30" t="str">
-        <v>Connect wires or components to each other</v>
+      <c r="D30" t="str">
+        <v>Heatshrink</v>
+      </c>
+      <c r="E30" t="str">
+        <v>https://uk.farnell.com/pro-power/pp3021/heatshrink-sleeving-kit-2-1-blk/dp/4161511?st=shrink%20tubing%20set</v>
+      </c>
+      <c r="F30" t="str">
+        <v>8.45</v>
+      </c>
+      <c r="G30" t="str">
+        <v>150pc</v>
+      </c>
+      <c r="J30" t="str">
+        <v>8.45</v>
       </c>
     </row>
     <row r="31">
-      <c r="D31" t="str">
-        <v>Ring terminal</v>
-      </c>
-      <c r="E31" t="str">
-        <v>https://uk.farnell.com/multicomp/crs-to-1806/terminal-ring-tongue-6-crimp/dp/1878197?st=wire%20to%20terminal%20connector</v>
-      </c>
-      <c r="F31" t="str">
-        <v>3.38</v>
-      </c>
-      <c r="G31" t="str">
-        <v>20pc</v>
-      </c>
-      <c r="J31" t="str">
-        <v>3.38</v>
+      <c r="B31" t="str">
+        <v>Boards</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Allow prototyping by placing components on a board</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="str">
-        <v>JST Female Connectors</v>
+        <v>150 Point Through Hole</v>
       </c>
       <c r="E32" t="str">
-        <v>https://uk.rs-online.com/web/p/circular-connector-contacts/6027900?gb=s</v>
+        <v>https://onecall.farnell.com/proto-advantage/sbbth1510-1/solder-breadboard-150-holes/dp/PC02483</v>
       </c>
       <c r="F32" t="str">
-        <v>4.70</v>
+        <v>5.97</v>
       </c>
       <c r="G32" t="str">
-        <v>50pc</v>
-      </c>
-      <c r="J32" t="str">
-        <v>4.70</v>
+        <v>3pc</v>
+      </c>
+      <c r="K32" t="str">
+        <v>5.97</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" t="str">
-        <v>JST Male Connectors</v>
+        <v>Breadboard Small</v>
       </c>
       <c r="E33" t="str">
-        <v>https://uk.rs-online.com/web/p/crimp-contacts/1613367?gb=s</v>
+        <v>https://onecall.farnell.com/cyntech/breadboard170red/breadboard-mini-red/dp/PC01594</v>
       </c>
       <c r="F33" t="str">
-        <v>3.40</v>
+        <v>4.11</v>
       </c>
       <c r="G33" t="str">
-        <v>100pc</v>
-      </c>
-      <c r="J33" t="str">
-        <v>3.40</v>
+        <v>3pc</v>
+      </c>
+      <c r="K33" t="str">
+        <v>4.11</v>
       </c>
     </row>
     <row r="34">
-      <c r="D34" t="str">
-        <v>Wire to board screw terminal single</v>
-      </c>
-      <c r="E34" t="str">
-        <v>https://uk.farnell.com/multicomp/mc000017/terminal-block-wire-to-brd-1pos/dp/2007984?st=screw%20terminal</v>
-      </c>
-      <c r="F34" t="str">
-        <v>8.12</v>
-      </c>
-      <c r="G34" t="str">
-        <v>20pc</v>
-      </c>
-      <c r="J34" t="str">
-        <v>8.12</v>
+      <c r="B34" t="str">
+        <v>Connectors</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Connect wires or components to each other</v>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="str">
-        <v>USB Female Breakout</v>
+        <v>Ring terminal</v>
       </c>
       <c r="E35" t="str">
-        <v>https://onecall.farnell.com/clever-little-box/cie-yy24/usb-2-0-a-socket-breakout-board/dp/CN22556</v>
+        <v>https://uk.farnell.com/multicomp/crs-to-1806/terminal-ring-tongue-6-crimp/dp/1878197?st=wire%20to%20terminal%20connector</v>
       </c>
       <c r="F35" t="str">
-        <v>5.10</v>
+        <v>3.38</v>
       </c>
       <c r="G35" t="str">
-        <v>5pc</v>
-      </c>
-      <c r="K35" t="str">
-        <v>5.10</v>
+        <v>20pc</v>
+      </c>
+      <c r="J35" t="str">
+        <v>3.38</v>
       </c>
     </row>
     <row r="36">
-      <c r="B36" t="str">
-        <v>Electronics</v>
-      </c>
-      <c r="C36" t="str">
-        <v>IRF520N</v>
+      <c r="D36" t="str">
+        <v>JST Female Connectors</v>
+      </c>
+      <c r="E36" t="str">
+        <v>https://uk.rs-online.com/web/p/circular-connector-contacts/6027900?gb=s</v>
+      </c>
+      <c r="F36" t="str">
+        <v>4.70</v>
+      </c>
+      <c r="G36" t="str">
+        <v>50pc</v>
+      </c>
+      <c r="J36" t="str">
+        <v>4.70</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" t="str">
-        <v>N Channel Mosfet to allow the Pi to control high voltage or high current components</v>
+        <v>JST Male Connectors</v>
       </c>
       <c r="E37" t="str">
-        <v>https://onecall.farnell.com/vishay/irf520pbf/mosfet-n-100v-9-2a-to-220/dp/8648239?st=irf520</v>
+        <v>https://uk.rs-online.com/web/p/crimp-contacts/1613367?gb=s</v>
       </c>
       <c r="F37" t="str">
-        <v>6.10</v>
+        <v>3.40</v>
       </c>
       <c r="G37" t="str">
-        <v>5pc</v>
-      </c>
-      <c r="K37" t="str">
-        <v>6.10</v>
+        <v>100pc</v>
+      </c>
+      <c r="J37" t="str">
+        <v>3.40</v>
       </c>
     </row>
     <row r="38">
-      <c r="B38" t="str">
-        <v>Transformers</v>
-      </c>
-      <c r="C38" t="str">
-        <v>Step down voltage</v>
+      <c r="D38" t="str">
+        <v>Wire to board screw terminal single</v>
+      </c>
+      <c r="E38" t="str">
+        <v>https://uk.farnell.com/multicomp/mc000017/terminal-block-wire-to-brd-1pos/dp/2007984?st=screw%20terminal</v>
+      </c>
+      <c r="F38" t="str">
+        <v>8.12</v>
+      </c>
+      <c r="G38" t="str">
+        <v>20pc</v>
+      </c>
+      <c r="J38" t="str">
+        <v>8.12</v>
       </c>
     </row>
     <row r="39">
       <c r="D39" t="str">
-        <v>24V 5A Max</v>
+        <v>USB Female Breakout</v>
       </c>
       <c r="E39" t="str">
-        <v>https://www.aliexpress.com/item/1005006174030695.html?spm=a2g0o.productlist.main.1.5afa5fddD8qxg0&amp;algo_pvid=6e377741-5938-4c8d-bf97-6cff92cf4000&amp;algo_exp_id=6e377741-5938-4c8d-bf97-6cff92cf4000-0&amp;pdp_npi=4%40dis%21GBP%215.41%211.78%21%21%2146.97%21%21%402103835c16995438817356700ed5d4%2112000036120896530%21sea%21UK%211802951889%21&amp;curPageLogUid=pZiqGrlJTVoB</v>
+        <v>https://onecall.farnell.com/clever-little-box/cie-yy24/usb-2-0-a-socket-breakout-board/dp/CN22556</v>
       </c>
       <c r="F39" t="str">
-        <v>9</v>
+        <v>5.10</v>
       </c>
       <c r="G39" t="str">
-        <v>5 pc</v>
+        <v>5pc</v>
+      </c>
+      <c r="K39" t="str">
+        <v>5.10</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="str">
-        <v>Screen</v>
-      </c>
       <c r="B40" t="str">
-        <v>HDMI Screen</v>
+        <v>Electronics</v>
       </c>
       <c r="C40" t="str">
-        <v>Display output using HDMI Connection</v>
+        <v>IRF520N</v>
       </c>
     </row>
     <row r="41">
       <c r="D41" t="str">
-        <v>DFROBOT DFR0506</v>
+        <v>N Channel Mosfet to allow the Pi to control high voltage or high current components</v>
       </c>
       <c r="E41" t="str">
-        <v>https://onecall.farnell.com/dfrobot/dfr0506/hdmi-display-embedded-dev-board/dp/3517851?st=hdmi%20screen</v>
+        <v>https://onecall.farnell.com/vishay/irf520pbf/mosfet-n-100v-9-2a-to-220/dp/8648239?st=irf520</v>
       </c>
       <c r="F41" t="str">
-        <v>65</v>
+        <v>6.10</v>
       </c>
       <c r="G41" t="str">
-        <v>7 Inch</v>
-      </c>
-      <c r="J41" t="str">
-        <v>65.29</v>
+        <v>5pc</v>
+      </c>
+      <c r="K41" t="str">
+        <v>6.10</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="str">
-        <v>Materials</v>
-      </c>
       <c r="B42" t="str">
-        <v>PETG</v>
+        <v>Transformers</v>
       </c>
       <c r="C42" t="str">
-        <v>Prototyping</v>
-      </c>
-      <c r="D42" t="str">
-        <v>Solid Grey</v>
-      </c>
-      <c r="E42" t="str">
-        <v>https://3dfilaprint.com/product/esun-petg-solid-grey-1-75mm-1kg-3d-printing-filament/</v>
-      </c>
-      <c r="F42" t="str">
-        <v>16</v>
-      </c>
-      <c r="G42" t="str">
-        <v>1kg</v>
-      </c>
-      <c r="J42" t="str">
-        <v>16</v>
+        <v>Step down voltage</v>
       </c>
     </row>
     <row r="43">
       <c r="D43" t="str">
+        <v>24V 5A Max</v>
+      </c>
+      <c r="E43" t="str">
+        <v>https://www.aliexpress.com/item/1005006174030695.html?spm=a2g0o.productlist.main.1.5afa5fddD8qxg0&amp;algo_pvid=6e377741-5938-4c8d-bf97-6cff92cf4000&amp;algo_exp_id=6e377741-5938-4c8d-bf97-6cff92cf4000-0&amp;pdp_npi=4%40dis%21GBP%215.41%211.78%21%21%2146.97%21%21%402103835c16995438817356700ed5d4%2112000036120896530%21sea%21UK%211802951889%21&amp;curPageLogUid=pZiqGrlJTVoB</v>
+      </c>
+      <c r="F43" t="str">
+        <v>9</v>
+      </c>
+      <c r="G43" t="str">
+        <v>5 pc</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Screen</v>
+      </c>
+      <c r="B44" t="str">
+        <v>HDMI Screen</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Display output using HDMI Connection</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="D45" t="str">
+        <v>DFROBOT DFR0506</v>
+      </c>
+      <c r="E45" t="str">
+        <v>https://onecall.farnell.com/dfrobot/dfr0506/hdmi-display-embedded-dev-board/dp/3517851?st=hdmi%20screen</v>
+      </c>
+      <c r="F45" t="str">
+        <v>65</v>
+      </c>
+      <c r="G45" t="str">
+        <v>7 Inch</v>
+      </c>
+      <c r="J45" t="str">
+        <v>65.29</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Materials</v>
+      </c>
+      <c r="B46" t="str">
+        <v>PETG</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Prototyping</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Solid Grey</v>
+      </c>
+      <c r="E46" t="str">
+        <v>https://3dfilaprint.com/product/esun-petg-solid-grey-1-75mm-1kg-3d-printing-filament/</v>
+      </c>
+      <c r="F46" t="str">
+        <v>16</v>
+      </c>
+      <c r="G46" t="str">
+        <v>1kg</v>
+      </c>
+      <c r="J46" t="str">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="D47" t="str">
         <v>Solid Black</v>
       </c>
-      <c r="E43" t="str">
+      <c r="E47" t="str">
         <v>https://3dfilaprint.com/product/esun-petg-solid-black-1-75mm-1kg-3d-printing-filament/</v>
       </c>
-      <c r="F43" t="str">
+      <c r="F47" t="str">
         <v>16</v>
       </c>
-      <c r="G43" t="str">
+      <c r="G47" t="str">
         <v>1kg</v>
       </c>
-      <c r="J43" t="str">
+      <c r="J47" t="str">
         <v>16</v>
       </c>
     </row>
-    <row r="44">
-      <c r="B44" t="str">
+    <row r="48">
+      <c r="B48" t="str">
         <v>Clear Plastic</v>
       </c>
-      <c r="C44" t="str">
+      <c r="C48" t="str">
         <v>For camera enclosure</v>
       </c>
-      <c r="D44" t="str">
+      <c r="D48" t="str">
         <v>Clear</v>
       </c>
-      <c r="E44" t="str">
+      <c r="E48" t="str">
         <v>https://uk.rs-online.com/web/p/plastic-sheets/0434295?gb=s</v>
       </c>
-      <c r="F44" t="str">
+      <c r="F48" t="str">
         <v>13.03</v>
       </c>
-      <c r="G44" t="str">
+      <c r="G48" t="str">
         <v>500x300x3mm</v>
       </c>
-      <c r="J44" t="str">
+      <c r="J48" t="str">
         <v>13.03</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q44"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q48"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>